<commit_message>
Solo falta lo de Excel, todo lo demas en teoria es funcional xd
</commit_message>
<xml_diff>
--- a/my-app/src/main/Resources/Libro1.xlsx
+++ b/my-app/src/main/Resources/Libro1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52834\Desktop\Leer Archivos\aperturaylecturadearchivos-DanielEDiaz\my-app\src\main\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A854027F-43F1-46D4-8007-F3E442DDCAE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D10A5-86DC-410E-A0B0-CCE7EDA3E90E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C130755-00D9-4BA6-A900-A661AF0721A4}"/>
+    <workbookView xWindow="3540" yWindow="4728" windowWidth="17280" windowHeight="8964" xr2:uid="{1C130755-00D9-4BA6-A900-A661AF0721A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Aulas" sheetId="1" r:id="rId1"/>
     <sheet name="Profesores" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,22 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Hola</t>
-  </si>
-  <si>
-    <t>Como</t>
-  </si>
-  <si>
-    <t>Estas</t>
-  </si>
-  <si>
-    <t>Yo</t>
-  </si>
-  <si>
-    <t>Bien</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Fulanito Martinez</t>
   </si>
@@ -60,13 +46,46 @@
     <t>BNM</t>
   </si>
   <si>
-    <t>Bruce Wayne</t>
-  </si>
-  <si>
-    <t>TYU</t>
-  </si>
-  <si>
-    <t>IOP</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Arturo Perez Reverte</t>
+  </si>
+  <si>
+    <t>QWE</t>
+  </si>
+  <si>
+    <t>RTY</t>
+  </si>
+  <si>
+    <t>A201-B</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>idk</t>
+  </si>
+  <si>
+    <t>E201</t>
+  </si>
+  <si>
+    <t>7845</t>
+  </si>
+  <si>
+    <t>A202-C</t>
+  </si>
+  <si>
+    <t>Salon</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>ayuda</t>
+  </si>
+  <si>
+    <t>me</t>
   </si>
 </sst>
 </file>
@@ -102,13 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,51 +439,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD510DA9-1B6B-427C-AC40-900BB8441DBA}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>8484</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>4599</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -478,40 +495,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AAABC0-27FF-4C54-8805-C41424516ECE}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4">
+      <c r="A1" s="1">
         <v>1546</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>6465</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDD5EE3-8F87-4708-A6E5-0DE3F70A2BBD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>